<commit_message>
Working version. Communication to serial worker more efficient. Gui states are tracked and graphs are only updated when focused. Frequency sweep information is tracked. Changed logic in the mainWorker to a simpler case statement with buffer dequeing.
</commit_message>
<xml_diff>
--- a/gui-breakdown.xlsx
+++ b/gui-breakdown.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Note</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Re-think layout (especially plots).</t>
   </si>
   <si>
-    <t>Look into communication between the serial thread and gui thread. Possible options ar portected buffers/variables r or  futures.</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
@@ -61,13 +58,19 @@
   </si>
   <si>
     <t>Note for Nick: Ensure that you can program/debug MCU - not high priority</t>
+  </si>
+  <si>
+    <t>http://fabienpn.wordpress.com/2013/08/16/qt-thread-multiple-methods-with-sources/</t>
+  </si>
+  <si>
+    <t>Look into communication between the serial thread and gui thread. Possible options are portected buffers/variables  or  futures.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +82,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,17 +112,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -411,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,68 +436,75 @@
     <col min="1" max="1" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="47.85546875" customWidth="1"/>
+    <col min="4" max="4" width="81.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>